<commit_message>
New classifications in Test Dataset
</commit_message>
<xml_diff>
--- a/skybrasil.xlsx
+++ b/skybrasil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vieir\Desktop\Insper\2° Semestre\CIÊNCIA DOS DADOS\Projeto 1\Projeto-1-CDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8428CF-CD97-4911-9668-8370A70658C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BF41A8-A648-42D5-9985-A8554C9ABE84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="755">
   <si>
     <t>Classificação</t>
   </si>
@@ -2579,9 +2579,6 @@
 quero cancelar
 nao aguento mais.. quero cancelar
 quero cancelar... cancelar... cancelar...</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2959,7 +2956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView topLeftCell="A493" workbookViewId="0">
+    <sheetView topLeftCell="A490" workbookViewId="0">
       <selection activeCell="A502" sqref="A502"/>
     </sheetView>
   </sheetViews>
@@ -6986,8 +6983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5362C36-A6BD-4474-811E-408B51E70798}">
   <dimension ref="A1:B253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7596,429 +7593,663 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>755</v>
+      <c r="A76">
+        <v>0</v>
       </c>
       <c r="B76" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>2</v>
+      </c>
       <c r="B77" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>2</v>
+      </c>
       <c r="B78" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>1</v>
+      </c>
       <c r="B79" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>2</v>
+      </c>
       <c r="B80" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>2</v>
+      </c>
       <c r="B81" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>0</v>
+      </c>
       <c r="B82" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>2</v>
+      </c>
       <c r="B83" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>2</v>
+      </c>
       <c r="B84" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>1</v>
+      </c>
       <c r="B85" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>1</v>
+      </c>
       <c r="B86" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>0</v>
+      </c>
       <c r="B87" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>1</v>
+      </c>
       <c r="B88" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>0</v>
+      </c>
       <c r="B89" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>2</v>
+      </c>
       <c r="B90" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>0</v>
+      </c>
       <c r="B91" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>2</v>
+      </c>
       <c r="B92" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>0</v>
+      </c>
       <c r="B93" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>1</v>
+      </c>
       <c r="B94" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>2</v>
+      </c>
       <c r="B95" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>2</v>
+      </c>
       <c r="B96" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>2</v>
+      </c>
       <c r="B97" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>1</v>
+      </c>
       <c r="B98" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>2</v>
+      </c>
       <c r="B99" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>2</v>
+      </c>
       <c r="B100" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>0</v>
+      </c>
       <c r="B101" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>0</v>
+      </c>
       <c r="B102" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>1</v>
+      </c>
       <c r="B103" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>1</v>
+      </c>
       <c r="B104" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>2</v>
+      </c>
       <c r="B105" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>2</v>
+      </c>
       <c r="B106" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>2</v>
+      </c>
       <c r="B107" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>2</v>
+      </c>
       <c r="B108" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>2</v>
+      </c>
       <c r="B109" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>2</v>
+      </c>
       <c r="B110" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>0</v>
+      </c>
       <c r="B111" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>2</v>
+      </c>
       <c r="B112" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>1</v>
+      </c>
       <c r="B113" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>2</v>
+      </c>
       <c r="B114" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>1</v>
+      </c>
       <c r="B115" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>0</v>
+      </c>
       <c r="B116" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>2</v>
+      </c>
       <c r="B117" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>1</v>
+      </c>
       <c r="B118" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>1</v>
+      </c>
       <c r="B119" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>2</v>
+      </c>
       <c r="B120" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>1</v>
+      </c>
       <c r="B121" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>2</v>
+      </c>
       <c r="B122" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>2</v>
+      </c>
       <c r="B123" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>0</v>
+      </c>
       <c r="B124" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>1</v>
+      </c>
       <c r="B125" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>0</v>
+      </c>
       <c r="B126" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>2</v>
+      </c>
       <c r="B127" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>2</v>
+      </c>
       <c r="B128" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>2</v>
+      </c>
       <c r="B129" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>2</v>
+      </c>
       <c r="B130" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>1</v>
+      </c>
       <c r="B131" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>2</v>
+      </c>
       <c r="B132" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>0</v>
+      </c>
       <c r="B133" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>1</v>
+      </c>
       <c r="B134" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>0</v>
+      </c>
       <c r="B135" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>0</v>
+      </c>
       <c r="B136" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>2</v>
+      </c>
       <c r="B137" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>2</v>
+      </c>
       <c r="B138" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>2</v>
+      </c>
       <c r="B139" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>2</v>
+      </c>
       <c r="B140" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>0</v>
+      </c>
       <c r="B141" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>1</v>
+      </c>
       <c r="B142" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>1</v>
+      </c>
       <c r="B143" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>1</v>
+      </c>
       <c r="B144" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>2</v>
+      </c>
       <c r="B145" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>0</v>
+      </c>
       <c r="B146" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>0</v>
+      </c>
       <c r="B147" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>2</v>
+      </c>
       <c r="B148" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>0</v>
+      </c>
       <c r="B149" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>1</v>
+      </c>
       <c r="B150" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>2</v>
+      </c>
       <c r="B151" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>1</v>
+      </c>
       <c r="B152" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>2</v>
+      </c>
       <c r="B153" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>2</v>
+      </c>
       <c r="B154" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B155" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B156" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B157" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B158" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B159" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B160" t="s">
         <v>661</v>
       </c>

</xml_diff>

<commit_message>
Classificator clear up Updated
</commit_message>
<xml_diff>
--- a/skybrasil.xlsx
+++ b/skybrasil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vieir\Desktop\Insper\2° Semestre\CIÊNCIA DOS DADOS\Projeto 1\Projeto-1-CDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B3E550-C04D-473C-9338-7108DA0DFDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35049F99-293A-4C8E-903E-83D90F5A00B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4332" yWindow="984" windowWidth="17280" windowHeight="11148" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -6992,8 +6992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5362C36-A6BD-4474-811E-408B51E70798}">
   <dimension ref="A1:B254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A244" sqref="A244"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7011,7 +7011,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>503</v>
@@ -7027,7 +7027,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>505</v>
@@ -7099,7 +7099,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>514</v>
@@ -7107,7 +7107,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
         <v>515</v>
@@ -7235,7 +7235,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
         <v>531</v>
@@ -7259,7 +7259,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
         <v>534</v>
@@ -7307,7 +7307,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B39" t="s">
         <v>540</v>
@@ -7323,7 +7323,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B41" t="s">
         <v>542</v>
@@ -7459,7 +7459,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B58" t="s">
         <v>559</v>
@@ -7515,7 +7515,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B65" t="s">
         <v>566</v>
@@ -7563,7 +7563,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B71" t="s">
         <v>572</v>
@@ -7571,7 +7571,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B72" t="s">
         <v>573</v>
@@ -7691,7 +7691,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B87" t="s">
         <v>588</v>
@@ -7723,7 +7723,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B91" t="s">
         <v>592</v>
@@ -8835,7 +8835,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B230" t="s">
         <v>731</v>
@@ -8859,7 +8859,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B233" t="s">
         <v>734</v>
@@ -8875,7 +8875,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B235" t="s">
         <v>736</v>
@@ -8947,7 +8947,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B244" t="s">
         <v>745</v>
@@ -8955,7 +8955,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B245" t="s">
         <v>746</v>

</xml_diff>

<commit_message>
Commits Finais para Entrega
</commit_message>
<xml_diff>
--- a/skybrasil.xlsx
+++ b/skybrasil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vieir\Desktop\Insper\2° Semestre\CIÊNCIA DOS DADOS\Projeto 1\Projeto-1-CDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F529482-2909-45E4-B05D-2D654B011E36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9403116C-96F6-4D49-8A7E-43FF9E1DA946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2965,8 +2965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="I183" sqref="I183"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>